<commit_message>
Traceability Matrix and S1 T2 PowerPoint Changes
See title.
</commit_message>
<xml_diff>
--- a/doc/Traceability Matrix/ChessGames Traceability Matrix.xlsx
+++ b/doc/Traceability Matrix/ChessGames Traceability Matrix.xlsx
@@ -311,7 +311,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -346,7 +346,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -648,15 +647,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB25"/>
+  <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection sqref="A1:L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -692,7 +691,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>11</v>
       </c>
@@ -710,7 +709,7 @@
       <c r="K2" s="13"/>
       <c r="L2" s="13"/>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>12</v>
       </c>
@@ -728,7 +727,7 @@
       <c r="K3" s="15"/>
       <c r="L3" s="15"/>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>13</v>
       </c>
@@ -746,7 +745,7 @@
       <c r="K4" s="17"/>
       <c r="L4" s="17"/>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>14</v>
       </c>
@@ -764,7 +763,7 @@
       <c r="K5" s="15"/>
       <c r="L5" s="15"/>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
         <v>15</v>
       </c>
@@ -782,7 +781,7 @@
       <c r="K6" s="17"/>
       <c r="L6" s="17"/>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>16</v>
       </c>
@@ -798,7 +797,7 @@
       <c r="K7" s="15"/>
       <c r="L7" s="15"/>
     </row>
-    <row r="8" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
         <v>17</v>
       </c>
@@ -813,24 +812,8 @@
       <c r="J8" s="17"/>
       <c r="K8" s="17"/>
       <c r="L8" s="17"/>
-      <c r="M8" s="18"/>
-      <c r="N8" s="18"/>
-      <c r="O8" s="18"/>
-      <c r="P8" s="18"/>
-      <c r="Q8" s="18"/>
-      <c r="R8" s="18"/>
-      <c r="S8" s="18"/>
-      <c r="T8" s="18"/>
-      <c r="U8" s="18"/>
-      <c r="V8" s="18"/>
-      <c r="W8" s="18"/>
-      <c r="X8" s="18"/>
-      <c r="Y8" s="18"/>
-      <c r="Z8" s="18"/>
-      <c r="AA8" s="18"/>
-      <c r="AB8" s="18"/>
-    </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>18</v>
       </c>
@@ -845,24 +828,8 @@
       <c r="J9" s="15"/>
       <c r="K9" s="15"/>
       <c r="L9" s="15"/>
-      <c r="M9" s="18"/>
-      <c r="N9" s="18"/>
-      <c r="O9" s="18"/>
-      <c r="P9" s="18"/>
-      <c r="Q9" s="18"/>
-      <c r="R9" s="18"/>
-      <c r="S9" s="18"/>
-      <c r="T9" s="18"/>
-      <c r="U9" s="18"/>
-      <c r="V9" s="18"/>
-      <c r="W9" s="18"/>
-      <c r="X9" s="18"/>
-      <c r="Y9" s="18"/>
-      <c r="Z9" s="18"/>
-      <c r="AA9" s="18"/>
-      <c r="AB9" s="18"/>
-    </row>
-    <row r="10" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
         <v>19</v>
       </c>
@@ -877,24 +844,8 @@
       <c r="J10" s="17"/>
       <c r="K10" s="17"/>
       <c r="L10" s="17"/>
-      <c r="M10" s="18"/>
-      <c r="N10" s="18"/>
-      <c r="O10" s="18"/>
-      <c r="P10" s="18"/>
-      <c r="Q10" s="18"/>
-      <c r="R10" s="18"/>
-      <c r="S10" s="18"/>
-      <c r="T10" s="18"/>
-      <c r="U10" s="18"/>
-      <c r="V10" s="18"/>
-      <c r="W10" s="18"/>
-      <c r="X10" s="18"/>
-      <c r="Y10" s="18"/>
-      <c r="Z10" s="18"/>
-      <c r="AA10" s="18"/>
-      <c r="AB10" s="18"/>
-    </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>20</v>
       </c>
@@ -909,24 +860,8 @@
       <c r="J11" s="15"/>
       <c r="K11" s="15"/>
       <c r="L11" s="15"/>
-      <c r="M11" s="18"/>
-      <c r="N11" s="18"/>
-      <c r="O11" s="18"/>
-      <c r="P11" s="18"/>
-      <c r="Q11" s="18"/>
-      <c r="R11" s="18"/>
-      <c r="S11" s="18"/>
-      <c r="T11" s="18"/>
-      <c r="U11" s="18"/>
-      <c r="V11" s="18"/>
-      <c r="W11" s="18"/>
-      <c r="X11" s="18"/>
-      <c r="Y11" s="18"/>
-      <c r="Z11" s="18"/>
-      <c r="AA11" s="18"/>
-      <c r="AB11" s="18"/>
-    </row>
-    <row r="12" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
         <v>21</v>
       </c>
@@ -941,24 +876,8 @@
       <c r="J12" s="17"/>
       <c r="K12" s="17"/>
       <c r="L12" s="17"/>
-      <c r="M12" s="18"/>
-      <c r="N12" s="18"/>
-      <c r="O12" s="18"/>
-      <c r="P12" s="18"/>
-      <c r="Q12" s="18"/>
-      <c r="R12" s="18"/>
-      <c r="S12" s="18"/>
-      <c r="T12" s="18"/>
-      <c r="U12" s="18"/>
-      <c r="V12" s="18"/>
-      <c r="W12" s="18"/>
-      <c r="X12" s="18"/>
-      <c r="Y12" s="18"/>
-      <c r="Z12" s="18"/>
-      <c r="AA12" s="18"/>
-      <c r="AB12" s="18"/>
-    </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>22</v>
       </c>
@@ -973,24 +892,8 @@
       <c r="J13" s="15"/>
       <c r="K13" s="15"/>
       <c r="L13" s="15"/>
-      <c r="M13" s="18"/>
-      <c r="N13" s="18"/>
-      <c r="O13" s="18"/>
-      <c r="P13" s="18"/>
-      <c r="Q13" s="18"/>
-      <c r="R13" s="18"/>
-      <c r="S13" s="18"/>
-      <c r="T13" s="18"/>
-      <c r="U13" s="18"/>
-      <c r="V13" s="18"/>
-      <c r="W13" s="18"/>
-      <c r="X13" s="18"/>
-      <c r="Y13" s="18"/>
-      <c r="Z13" s="18"/>
-      <c r="AA13" s="18"/>
-      <c r="AB13" s="18"/>
-    </row>
-    <row r="14" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
         <v>23</v>
       </c>
@@ -1005,24 +908,8 @@
       <c r="J14" s="17"/>
       <c r="K14" s="17"/>
       <c r="L14" s="17"/>
-      <c r="M14" s="18"/>
-      <c r="N14" s="18"/>
-      <c r="O14" s="18"/>
-      <c r="P14" s="18"/>
-      <c r="Q14" s="18"/>
-      <c r="R14" s="18"/>
-      <c r="S14" s="18"/>
-      <c r="T14" s="18"/>
-      <c r="U14" s="18"/>
-      <c r="V14" s="18"/>
-      <c r="W14" s="18"/>
-      <c r="X14" s="18"/>
-      <c r="Y14" s="18"/>
-      <c r="Z14" s="18"/>
-      <c r="AA14" s="18"/>
-      <c r="AB14" s="18"/>
-    </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
         <v>24</v>
       </c>
@@ -1039,24 +926,8 @@
       <c r="J15" s="15"/>
       <c r="K15" s="15"/>
       <c r="L15" s="15"/>
-      <c r="M15" s="18"/>
-      <c r="N15" s="18"/>
-      <c r="O15" s="18"/>
-      <c r="P15" s="18"/>
-      <c r="Q15" s="18"/>
-      <c r="R15" s="18"/>
-      <c r="S15" s="18"/>
-      <c r="T15" s="18"/>
-      <c r="U15" s="18"/>
-      <c r="V15" s="18"/>
-      <c r="W15" s="18"/>
-      <c r="X15" s="18"/>
-      <c r="Y15" s="18"/>
-      <c r="Z15" s="18"/>
-      <c r="AA15" s="18"/>
-      <c r="AB15" s="18"/>
-    </row>
-    <row r="16" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
         <v>25</v>
       </c>
@@ -1071,24 +942,8 @@
       <c r="J16" s="17"/>
       <c r="K16" s="17"/>
       <c r="L16" s="17"/>
-      <c r="M16" s="18"/>
-      <c r="N16" s="18"/>
-      <c r="O16" s="18"/>
-      <c r="P16" s="18"/>
-      <c r="Q16" s="18"/>
-      <c r="R16" s="18"/>
-      <c r="S16" s="18"/>
-      <c r="T16" s="18"/>
-      <c r="U16" s="18"/>
-      <c r="V16" s="18"/>
-      <c r="W16" s="18"/>
-      <c r="X16" s="18"/>
-      <c r="Y16" s="18"/>
-      <c r="Z16" s="18"/>
-      <c r="AA16" s="18"/>
-      <c r="AB16" s="18"/>
-    </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>26</v>
       </c>
@@ -1103,24 +958,8 @@
       <c r="J17" s="15"/>
       <c r="K17" s="15"/>
       <c r="L17" s="15"/>
-      <c r="M17" s="18"/>
-      <c r="N17" s="18"/>
-      <c r="O17" s="18"/>
-      <c r="P17" s="18"/>
-      <c r="Q17" s="18"/>
-      <c r="R17" s="18"/>
-      <c r="S17" s="18"/>
-      <c r="T17" s="18"/>
-      <c r="U17" s="18"/>
-      <c r="V17" s="18"/>
-      <c r="W17" s="18"/>
-      <c r="X17" s="18"/>
-      <c r="Y17" s="18"/>
-      <c r="Z17" s="18"/>
-      <c r="AA17" s="18"/>
-      <c r="AB17" s="18"/>
-    </row>
-    <row r="18" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
         <v>27</v>
       </c>
@@ -1135,24 +974,8 @@
       <c r="J18" s="17"/>
       <c r="K18" s="17"/>
       <c r="L18" s="17"/>
-      <c r="M18" s="18"/>
-      <c r="N18" s="18"/>
-      <c r="O18" s="18"/>
-      <c r="P18" s="18"/>
-      <c r="Q18" s="18"/>
-      <c r="R18" s="18"/>
-      <c r="S18" s="18"/>
-      <c r="T18" s="18"/>
-      <c r="U18" s="18"/>
-      <c r="V18" s="18"/>
-      <c r="W18" s="18"/>
-      <c r="X18" s="18"/>
-      <c r="Y18" s="18"/>
-      <c r="Z18" s="18"/>
-      <c r="AA18" s="18"/>
-      <c r="AB18" s="18"/>
-    </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
         <v>28</v>
       </c>
@@ -1167,24 +990,8 @@
       <c r="J19" s="15"/>
       <c r="K19" s="15"/>
       <c r="L19" s="15"/>
-      <c r="M19" s="18"/>
-      <c r="N19" s="18"/>
-      <c r="O19" s="18"/>
-      <c r="P19" s="18"/>
-      <c r="Q19" s="18"/>
-      <c r="R19" s="18"/>
-      <c r="S19" s="18"/>
-      <c r="T19" s="18"/>
-      <c r="U19" s="18"/>
-      <c r="V19" s="18"/>
-      <c r="W19" s="18"/>
-      <c r="X19" s="18"/>
-      <c r="Y19" s="18"/>
-      <c r="Z19" s="18"/>
-      <c r="AA19" s="18"/>
-      <c r="AB19" s="18"/>
-    </row>
-    <row r="20" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="9">
         <v>8</v>
       </c>
@@ -1199,24 +1006,8 @@
       <c r="J20" s="17"/>
       <c r="K20" s="17"/>
       <c r="L20" s="17"/>
-      <c r="M20" s="18"/>
-      <c r="N20" s="18"/>
-      <c r="O20" s="18"/>
-      <c r="P20" s="18"/>
-      <c r="Q20" s="18"/>
-      <c r="R20" s="18"/>
-      <c r="S20" s="18"/>
-      <c r="T20" s="18"/>
-      <c r="U20" s="18"/>
-      <c r="V20" s="18"/>
-      <c r="W20" s="18"/>
-      <c r="X20" s="18"/>
-      <c r="Y20" s="18"/>
-      <c r="Z20" s="18"/>
-      <c r="AA20" s="18"/>
-      <c r="AB20" s="18"/>
-    </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="10">
         <v>9</v>
       </c>
@@ -1231,24 +1022,8 @@
       <c r="J21" s="15"/>
       <c r="K21" s="15"/>
       <c r="L21" s="15"/>
-      <c r="M21" s="18"/>
-      <c r="N21" s="18"/>
-      <c r="O21" s="18"/>
-      <c r="P21" s="18"/>
-      <c r="Q21" s="18"/>
-      <c r="R21" s="18"/>
-      <c r="S21" s="18"/>
-      <c r="T21" s="18"/>
-      <c r="U21" s="18"/>
-      <c r="V21" s="18"/>
-      <c r="W21" s="18"/>
-      <c r="X21" s="18"/>
-      <c r="Y21" s="18"/>
-      <c r="Z21" s="18"/>
-      <c r="AA21" s="18"/>
-      <c r="AB21" s="18"/>
-    </row>
-    <row r="22" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="9">
         <v>10</v>
       </c>
@@ -1263,24 +1038,8 @@
       <c r="J22" s="17"/>
       <c r="K22" s="17"/>
       <c r="L22" s="17"/>
-      <c r="M22" s="18"/>
-      <c r="N22" s="18"/>
-      <c r="O22" s="18"/>
-      <c r="P22" s="18"/>
-      <c r="Q22" s="18"/>
-      <c r="R22" s="18"/>
-      <c r="S22" s="18"/>
-      <c r="T22" s="18"/>
-      <c r="U22" s="18"/>
-      <c r="V22" s="18"/>
-      <c r="W22" s="18"/>
-      <c r="X22" s="18"/>
-      <c r="Y22" s="18"/>
-      <c r="Z22" s="18"/>
-      <c r="AA22" s="18"/>
-      <c r="AB22" s="18"/>
-    </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" s="10">
         <v>11</v>
       </c>
@@ -1295,24 +1054,8 @@
       <c r="J23" s="15"/>
       <c r="K23" s="15"/>
       <c r="L23" s="15"/>
-      <c r="M23" s="18"/>
-      <c r="N23" s="18"/>
-      <c r="O23" s="18"/>
-      <c r="P23" s="18"/>
-      <c r="Q23" s="18"/>
-      <c r="R23" s="18"/>
-      <c r="S23" s="18"/>
-      <c r="T23" s="18"/>
-      <c r="U23" s="18"/>
-      <c r="V23" s="18"/>
-      <c r="W23" s="18"/>
-      <c r="X23" s="18"/>
-      <c r="Y23" s="18"/>
-      <c r="Z23" s="18"/>
-      <c r="AA23" s="18"/>
-      <c r="AB23" s="18"/>
-    </row>
-    <row r="24" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="9">
         <v>12</v>
       </c>
@@ -1331,24 +1074,8 @@
       <c r="J24" s="17"/>
       <c r="K24" s="17"/>
       <c r="L24" s="17"/>
-      <c r="M24" s="18"/>
-      <c r="N24" s="18"/>
-      <c r="O24" s="18"/>
-      <c r="P24" s="18"/>
-      <c r="Q24" s="18"/>
-      <c r="R24" s="18"/>
-      <c r="S24" s="18"/>
-      <c r="T24" s="18"/>
-      <c r="U24" s="18"/>
-      <c r="V24" s="18"/>
-      <c r="W24" s="18"/>
-      <c r="X24" s="18"/>
-      <c r="Y24" s="18"/>
-      <c r="Z24" s="18"/>
-      <c r="AA24" s="18"/>
-      <c r="AB24" s="18"/>
-    </row>
-    <row r="25" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="25" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="11" t="s">
         <v>29</v>
       </c>

</xml_diff>